<commit_message>
long time ago in a galaxy far away
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merca\Desktop\diadema_ajmc2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3EE67F-717A-40A8-8B21-9D7EEEEFA9A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4628C2-CD1B-40D4-BFF4-FEA2D2950B18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2628" yWindow="1146" windowWidth="17280" windowHeight="9102" activeTab="4" xr2:uid="{A63E299C-D04E-45E4-B40C-A232108876F3}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" activeTab="2" xr2:uid="{A63E299C-D04E-45E4-B40C-A232108876F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Site Description" sheetId="3" r:id="rId1"/>
@@ -633,19 +633,22 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -654,13 +657,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -694,90 +694,33 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Sea Urchin</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Collected by Size &amp; Municipality in Puerto Rico</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="5"/>
+          <c:idx val="7"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Collection!$B$1</c:f>
+              <c:f>Collection!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.5 in</c:v>
+                  <c:v>Ceiba</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -787,64 +730,52 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Collection!$A$2:$A$9</c:f>
+              <c:f>Collection!$B$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Rincon</c:v>
+                  <c:v>1.5 in</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Ponce</c:v>
+                  <c:v>2 in</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Luquillo</c:v>
+                  <c:v>2.5 in</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Isabela</c:v>
+                  <c:v>3 in</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Guayama</c:v>
+                  <c:v>3.5 in</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Guanica</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Culebra</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ceiba</c:v>
+                  <c:v>4.5 in</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Collection!$B$2:$B$9</c:f>
+              <c:f>Collection!$B$9:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -852,20 +783,442 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-8A02-4314-A870-3606AE7C6F43}"/>
+              <c16:uniqueId val="{00000002-ECCA-4B2E-8260-5F8EAE42C9C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Collection!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Culebra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Collection!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5 in</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 in</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5 in</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 in</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5 in</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5 in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Collection!$B$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ECCA-4B2E-8260-5F8EAE42C9C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Collection!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Guanica</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Collection!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5 in</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 in</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5 in</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 in</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5 in</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5 in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Collection!$B$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8A02-4314-A870-3606AE7C6F43}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Collection!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Guayama</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Collection!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5 in</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 in</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5 in</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 in</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5 in</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5 in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Collection!$B$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8A02-4314-A870-3606AE7C6F43}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Collection!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Isabela</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Collection!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5 in</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 in</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5 in</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 in</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5 in</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5 in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Collection!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8A02-4314-A870-3606AE7C6F43}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Collection!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Luquillo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Collection!$B$1:$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5 in</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 in</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5 in</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3 in</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5 in</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5 in</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Collection!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8A02-4314-A870-3606AE7C6F43}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="1"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Collection!$C$1</c:f>
+              <c:f>Collection!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 in</c:v>
+                  <c:v>Ponce</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -882,44 +1235,38 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Collection!$A$2:$A$9</c:f>
+              <c:f>Collection!$B$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Rincon</c:v>
+                  <c:v>1.5 in</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Ponce</c:v>
+                  <c:v>2 in</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Luquillo</c:v>
+                  <c:v>2.5 in</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Isabela</c:v>
+                  <c:v>3 in</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Guayama</c:v>
+                  <c:v>3.5 in</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Guanica</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Culebra</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ceiba</c:v>
+                  <c:v>4.5 in</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Collection!$C$2:$C$9</c:f>
+              <c:f>Collection!$B$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -928,19 +1275,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -952,22 +1293,24 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:idx val="5"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Collection!$D$1</c:f>
+              <c:f>Collection!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5 in</c:v>
+                  <c:v>Rincon</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -977,357 +1320,60 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Collection!$A$2:$A$9</c:f>
+              <c:f>Collection!$B$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Rincon</c:v>
+                  <c:v>1.5 in</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Ponce</c:v>
+                  <c:v>2 in</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Luquillo</c:v>
+                  <c:v>2.5 in</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Isabela</c:v>
+                  <c:v>3 in</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Guayama</c:v>
+                  <c:v>3.5 in</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Guanica</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Culebra</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ceiba</c:v>
+                  <c:v>4.5 in</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Collection!$D$2:$D$9</c:f>
+              <c:f>Collection!$B$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8A02-4314-A870-3606AE7C6F43}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Collection!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3 in</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Collection!$A$2:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Rincon</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ponce</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Luquillo</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Isabela</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Guayama</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Guanica</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Culebra</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ceiba</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Collection!$E$2:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8A02-4314-A870-3606AE7C6F43}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Collection!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3.5 in</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Collection!$A$2:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Rincon</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ponce</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Luquillo</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Isabela</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Guayama</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Guanica</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Culebra</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ceiba</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Collection!$F$2:$F$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8A02-4314-A870-3606AE7C6F43}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Collection!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>4.5 in</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Collection!$A$2:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>Rincon</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ponce</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Luquillo</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Isabela</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Guayama</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Guanica</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Culebra</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Ceiba</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Collection!$G$2:$G$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-8A02-4314-A870-3606AE7C6F43}"/>
+              <c16:uniqueId val="{00000006-8A02-4314-A870-3606AE7C6F43}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1340,7 +1386,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
         <c:axId val="473471760"/>
         <c:axId val="473466184"/>
       </c:barChart>
@@ -1350,7 +1395,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1401,7 +1446,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1432,7 +1477,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1474,7 +1519,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1492,7 +1537,7 @@
       </c:dTable>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -2147,13 +2192,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -3781,16 +3823,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>203836</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>46672</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4239,186 +4281,194 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="237.3" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="20" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="12"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" ht="405.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="17" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="12"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4" ht="136.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="12"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="352.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="67.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:4" ht="254.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A11" s="12"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4" ht="287.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="17" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A13" s="12"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="117.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="14" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="67.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="19"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:4" ht="67.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="12"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4" ht="405.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="17" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A18" s="12"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
@@ -4427,21 +4477,13 @@
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5377,8 +5419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7FF494F-F1FA-4556-AFEA-3AB47A5A9B7D}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="B1:G9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5737,7 +5779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A43E6FBF-F068-46E2-93D6-F5F9E960854B}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>